<commit_message>
Finalized and Proofread WarIsComing Story
</commit_message>
<xml_diff>
--- a/Stories/WarIsComing.xlsx
+++ b/Stories/WarIsComing.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="I:\DECO3801-Synergistiscs\Stories\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ianch\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{ACE0122B-6FDB-4BFA-A272-11EB014B71DB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B04E654D-AE43-457D-83F4-67D74EFA7D4E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{4C62B3AD-FD19-43ED-8515-0095E96B2E3E}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{4C62B3AD-FD19-43ED-8515-0095E96B2E3E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -92,30 +92,15 @@
     <t>War is coming?</t>
   </si>
   <si>
-    <t>Multiple reports from kingom scouts have reported an unusual amount of military activity in a neighbouring country. Numbers show has many as 5,000 young men have returned from other duties and missions by command of their king. An increase in smoke in the area, scientists believe to be linked to an increase in blacksmithing.</t>
-  </si>
-  <si>
     <t>ADVISOR OPINION</t>
   </si>
   <si>
-    <t>There was serious tension at the last ally meeting of commanders.</t>
-  </si>
-  <si>
     <t>My troops at the border have also noticed more 'friendly' scouts than usual in the area.</t>
   </si>
   <si>
     <t>We haven't had a war in over 100 years, history shows another war may be due.</t>
   </si>
   <si>
-    <t>If history has taught us anything its that we must strike first</t>
-  </si>
-  <si>
-    <t>We need to stop trading with them immediately, in the past this has slowed down war.</t>
-  </si>
-  <si>
-    <t>By my accounts we have been exporting more food than usual there.</t>
-  </si>
-  <si>
     <t>If we are going to war, we may not have enough to hold off for a long period.</t>
   </si>
   <si>
@@ -128,18 +113,9 @@
     <t xml:space="preserve">There are reports of our neighbouring Kingdoms recruiting blacksmith talents. </t>
   </si>
   <si>
-    <t>My job is to create diplomatic ftiendships with neighbouring Kingdom, not making wars.</t>
-  </si>
-  <si>
-    <t>I guess it is time to request assistance from our allies!</t>
-  </si>
-  <si>
     <t>OUTCOME</t>
   </si>
   <si>
-    <t>The reports are confirmed. The neighbouring kingom is amassing troops and it appears a war is coming.</t>
-  </si>
-  <si>
     <t>ACTION 1</t>
   </si>
   <si>
@@ -179,9 +155,6 @@
     <t>This is too optimistic!</t>
   </si>
   <si>
-    <t>Are not we responsible to come up with a plan in times like this?</t>
-  </si>
-  <si>
     <t>ACTION 2</t>
   </si>
   <si>
@@ -191,15 +164,6 @@
     <t>We are unprepared, defence at this point may be our best attack</t>
   </si>
   <si>
-    <t>We must catch them off guard.</t>
-  </si>
-  <si>
-    <t>From reports, attacking first uses more resources.</t>
-  </si>
-  <si>
-    <t>In my opinion attacking first is always the best move.</t>
-  </si>
-  <si>
     <t>We should all hide.</t>
   </si>
   <si>
@@ -233,24 +197,12 @@
     <t>We will face retaliation.</t>
   </si>
   <si>
-    <t>No food, no troops</t>
-  </si>
-  <si>
     <t>We should raise the prices.</t>
   </si>
   <si>
-    <t>Reports show our wealth will drop.</t>
-  </si>
-  <si>
     <t>We should save our own food.</t>
   </si>
   <si>
-    <t>We will be leaving many children to starve</t>
-  </si>
-  <si>
-    <t>There will be excessive surplus that leads to wastage.</t>
-  </si>
-  <si>
     <t>This will cause economy stagnation that reduces the Kingdom incomes.</t>
   </si>
   <si>
@@ -275,9 +227,6 @@
     <t>We should protect those needed for rebuilding.</t>
   </si>
   <si>
-    <t>This is a weak move.</t>
-  </si>
-  <si>
     <t>Great idea... if I come too.</t>
   </si>
   <si>
@@ -293,15 +242,9 @@
     <t>I do not see any harm doing this.</t>
   </si>
   <si>
-    <t xml:space="preserve">AT least we can protect the people lives and properties. </t>
-  </si>
-  <si>
     <t>The fortification is only temporary. We still have to end the war.</t>
   </si>
   <si>
-    <t>This is a move that could save our people, but not the Kingdom.</t>
-  </si>
-  <si>
     <t>There would not be enough time to evacuate all the people.</t>
   </si>
   <si>
@@ -309,6 +252,63 @@
   </si>
   <si>
     <t>MONASTERY</t>
+  </si>
+  <si>
+    <t>There was serious tension at the last ally meeting with the commanders.</t>
+  </si>
+  <si>
+    <t>If history has taught us anything, it's that we must strike first.</t>
+  </si>
+  <si>
+    <t>We need to stop trading with them immediately. In the past, this has slowed down war.</t>
+  </si>
+  <si>
+    <t>By my accounts, we have been exporting more food than usual there.</t>
+  </si>
+  <si>
+    <t>My job is to create diplomatic friendships with neighbouring Kingdom, not making wars.</t>
+  </si>
+  <si>
+    <t>I guess it's the time to request assistance from our allies!</t>
+  </si>
+  <si>
+    <t>The reports are confirmed. The neighbouring Kingdom is amassing troops and it appears a war is coming.</t>
+  </si>
+  <si>
+    <t>Multiple reports from the Kingdom scouts have reported an unusual amount of military activities in a neighbouring Kingdom. Numbers has shown as many as 5,000 young men have returned from other duties and missions by their king command's. More smoke has been sighted in the area, scientists believed there are linked to an increase in blacksmithing.</t>
+  </si>
+  <si>
+    <t>Aren't we advisors responsible to come up with a plan in times like this?</t>
+  </si>
+  <si>
+    <t>We must catch them off guard!</t>
+  </si>
+  <si>
+    <t>From most war reports, attacking first uses more resources.</t>
+  </si>
+  <si>
+    <t>In my opinion, attacking first is always the best move.</t>
+  </si>
+  <si>
+    <t>No food, no troops.</t>
+  </si>
+  <si>
+    <t>The forecast report shows that our wealth will drop.</t>
+  </si>
+  <si>
+    <t>We will be leaving many children to starve.</t>
+  </si>
+  <si>
+    <t>There will be excessive surplus that leads to food wastage.</t>
+  </si>
+  <si>
+    <t>This is a weak move!</t>
+  </si>
+  <si>
+    <t xml:space="preserve">At least we can protect the people lives and properties. </t>
+  </si>
+  <si>
+    <t>This is a move that could save our people, but losing the Kingdom.</t>
   </si>
 </sst>
 </file>
@@ -488,13 +488,6 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -529,10 +522,14 @@
     <xf numFmtId="0" fontId="7" fillId="6" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="5" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -547,8 +544,11 @@
     <xf numFmtId="0" fontId="6" fillId="5" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -867,418 +867,424 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C44981BA-9AE4-44E2-B14F-CB86D6B680A9}">
   <dimension ref="A1:M14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="M14" sqref="M14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1" s="1"/>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="3"/>
-      <c r="D1" s="4" t="s">
+      <c r="C1" s="17"/>
+      <c r="D1" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="3"/>
-      <c r="F1" s="4" t="s">
+      <c r="E1" s="17"/>
+      <c r="F1" s="25" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="3"/>
-      <c r="H1" s="4" t="s">
+      <c r="G1" s="17"/>
+      <c r="H1" s="25" t="s">
         <v>3</v>
       </c>
-      <c r="I1" s="3"/>
-      <c r="J1" s="4" t="s">
+      <c r="I1" s="17"/>
+      <c r="J1" s="25" t="s">
         <v>4</v>
       </c>
-      <c r="K1" s="3"/>
-      <c r="L1" s="4" t="s">
+      <c r="K1" s="17"/>
+      <c r="L1" s="25" t="s">
         <v>5</v>
       </c>
-      <c r="M1" s="3"/>
-    </row>
-    <row r="2" spans="1:13" ht="42.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="5"/>
-      <c r="B2" s="6" t="s">
+      <c r="M1" s="17"/>
+    </row>
+    <row r="2" spans="1:13" ht="41.4" x14ac:dyDescent="0.3">
+      <c r="A2" s="2"/>
+      <c r="B2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="C2" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="7" t="s">
+      <c r="D2" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="7" t="s">
+      <c r="E2" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="F2" s="7" t="s">
+      <c r="F2" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="G2" s="7" t="s">
+      <c r="G2" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="H2" s="7" t="s">
+      <c r="H2" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="I2" s="7" t="s">
+      <c r="I2" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="J2" s="7" t="s">
+      <c r="J2" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="K2" s="7" t="s">
+      <c r="K2" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="L2" s="7" t="s">
+      <c r="L2" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="M2" s="7" t="s">
+      <c r="M2" s="4" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="25" t="s">
+    <row r="3" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="14" t="s">
+        <v>72</v>
+      </c>
+      <c r="B3" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="C3" s="16"/>
+      <c r="D3" s="16"/>
+      <c r="E3" s="16"/>
+      <c r="F3" s="16"/>
+      <c r="G3" s="16"/>
+      <c r="H3" s="16"/>
+      <c r="I3" s="16"/>
+      <c r="J3" s="16"/>
+      <c r="K3" s="16"/>
+      <c r="L3" s="16"/>
+      <c r="M3" s="17"/>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A4" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="B4" s="19" t="s">
+        <v>80</v>
+      </c>
+      <c r="C4" s="16"/>
+      <c r="D4" s="16"/>
+      <c r="E4" s="16"/>
+      <c r="F4" s="16"/>
+      <c r="G4" s="16"/>
+      <c r="H4" s="16"/>
+      <c r="I4" s="16"/>
+      <c r="J4" s="16"/>
+      <c r="K4" s="16"/>
+      <c r="L4" s="16"/>
+      <c r="M4" s="17"/>
+    </row>
+    <row r="5" spans="1:13" ht="180" x14ac:dyDescent="0.3">
+      <c r="A5" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="E5" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="F5" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="G5" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="H5" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="I5" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="J5" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="K5" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="L5" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="M5" s="7" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" ht="28.2" x14ac:dyDescent="0.3">
+      <c r="A6" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="B6" s="20" t="s">
+        <v>79</v>
+      </c>
+      <c r="C6" s="21"/>
+      <c r="D6" s="21"/>
+      <c r="E6" s="21"/>
+      <c r="F6" s="21"/>
+      <c r="G6" s="21"/>
+      <c r="H6" s="21"/>
+      <c r="I6" s="21"/>
+      <c r="J6" s="21"/>
+      <c r="K6" s="21"/>
+      <c r="L6" s="21"/>
+      <c r="M6" s="22"/>
+    </row>
+    <row r="7" spans="1:13" ht="28.2" x14ac:dyDescent="0.3">
+      <c r="A7" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="B7" s="23" t="s">
+        <v>28</v>
+      </c>
+      <c r="C7" s="16"/>
+      <c r="D7" s="16"/>
+      <c r="E7" s="16"/>
+      <c r="F7" s="16"/>
+      <c r="G7" s="16"/>
+      <c r="H7" s="16"/>
+      <c r="I7" s="16"/>
+      <c r="J7" s="16"/>
+      <c r="K7" s="16"/>
+      <c r="L7" s="16"/>
+      <c r="M7" s="17"/>
+    </row>
+    <row r="8" spans="1:13" ht="138.6" x14ac:dyDescent="0.3">
+      <c r="A8" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="C8" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="D8" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="E8" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="F8" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="G8" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="H8" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="I8" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="J8" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="K8" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="L8" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="M8" s="7" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" ht="28.2" x14ac:dyDescent="0.3">
+      <c r="A9" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="B9" s="18" t="s">
+        <v>41</v>
+      </c>
+      <c r="C9" s="16"/>
+      <c r="D9" s="16"/>
+      <c r="E9" s="16"/>
+      <c r="F9" s="16"/>
+      <c r="G9" s="16"/>
+      <c r="H9" s="16"/>
+      <c r="I9" s="16"/>
+      <c r="J9" s="16"/>
+      <c r="K9" s="16"/>
+      <c r="L9" s="16"/>
+      <c r="M9" s="17"/>
+    </row>
+    <row r="10" spans="1:13" ht="152.4" x14ac:dyDescent="0.3">
+      <c r="A10" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="C10" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="D10" s="7" t="s">
+        <v>83</v>
+      </c>
+      <c r="E10" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="F10" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="G10" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="H10" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="I10" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="J10" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="K10" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="L10" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="M10" s="7" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" ht="28.2" x14ac:dyDescent="0.3">
+      <c r="A11" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="B11" s="18" t="s">
+        <v>52</v>
+      </c>
+      <c r="C11" s="16"/>
+      <c r="D11" s="16"/>
+      <c r="E11" s="16"/>
+      <c r="F11" s="16"/>
+      <c r="G11" s="16"/>
+      <c r="H11" s="16"/>
+      <c r="I11" s="16"/>
+      <c r="J11" s="16"/>
+      <c r="K11" s="16"/>
+      <c r="L11" s="16"/>
+      <c r="M11" s="17"/>
+    </row>
+    <row r="12" spans="1:13" ht="180" x14ac:dyDescent="0.3">
+      <c r="A12" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="B12" s="12" t="s">
+        <v>53</v>
+      </c>
+      <c r="C12" s="13" t="s">
+        <v>85</v>
+      </c>
+      <c r="D12" s="13" t="s">
+        <v>54</v>
+      </c>
+      <c r="E12" s="13" t="s">
+        <v>86</v>
+      </c>
+      <c r="F12" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="G12" s="12" t="s">
+        <v>87</v>
+      </c>
+      <c r="H12" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="I12" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="J12" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="K12" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="L12" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="M12" s="7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" ht="28.2" x14ac:dyDescent="0.3">
+      <c r="A13" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="B13" s="18" t="s">
+        <v>62</v>
+      </c>
+      <c r="C13" s="16"/>
+      <c r="D13" s="16"/>
+      <c r="E13" s="16"/>
+      <c r="F13" s="16"/>
+      <c r="G13" s="16"/>
+      <c r="H13" s="16"/>
+      <c r="I13" s="16"/>
+      <c r="J13" s="16"/>
+      <c r="K13" s="16"/>
+      <c r="L13" s="16"/>
+      <c r="M13" s="17"/>
+    </row>
+    <row r="14" spans="1:13" ht="152.4" x14ac:dyDescent="0.3">
+      <c r="A14" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="B14" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="C14" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="D14" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="E14" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="F14" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="G14" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="H14" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="I14" s="7" t="s">
+        <v>90</v>
+      </c>
+      <c r="J14" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="K14" s="7" t="s">
         <v>91</v>
       </c>
-      <c r="B3" s="17" t="s">
-        <v>18</v>
-      </c>
-      <c r="C3" s="18"/>
-      <c r="D3" s="18"/>
-      <c r="E3" s="18"/>
-      <c r="F3" s="18"/>
-      <c r="G3" s="18"/>
-      <c r="H3" s="18"/>
-      <c r="I3" s="18"/>
-      <c r="J3" s="18"/>
-      <c r="K3" s="18"/>
-      <c r="L3" s="18"/>
-      <c r="M3" s="3"/>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A4" s="8" t="b">
-        <v>1</v>
-      </c>
-      <c r="B4" s="20" t="s">
-        <v>19</v>
-      </c>
-      <c r="C4" s="18"/>
-      <c r="D4" s="18"/>
-      <c r="E4" s="18"/>
-      <c r="F4" s="18"/>
-      <c r="G4" s="18"/>
-      <c r="H4" s="18"/>
-      <c r="I4" s="18"/>
-      <c r="J4" s="18"/>
-      <c r="K4" s="18"/>
-      <c r="L4" s="18"/>
-      <c r="M4" s="3"/>
-    </row>
-    <row r="5" spans="1:13" ht="186" x14ac:dyDescent="0.25">
-      <c r="A5" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="B5" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="C5" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="D5" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="E5" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="F5" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="G5" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="H5" s="10" t="s">
-        <v>27</v>
-      </c>
-      <c r="I5" s="10" t="s">
-        <v>28</v>
-      </c>
-      <c r="J5" s="10" t="s">
-        <v>29</v>
-      </c>
-      <c r="K5" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="L5" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="M5" s="10" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13" ht="29.25" x14ac:dyDescent="0.25">
-      <c r="A6" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="B6" s="21" t="s">
-        <v>34</v>
-      </c>
-      <c r="C6" s="22"/>
-      <c r="D6" s="22"/>
-      <c r="E6" s="22"/>
-      <c r="F6" s="22"/>
-      <c r="G6" s="22"/>
-      <c r="H6" s="22"/>
-      <c r="I6" s="22"/>
-      <c r="J6" s="22"/>
-      <c r="K6" s="22"/>
-      <c r="L6" s="22"/>
-      <c r="M6" s="23"/>
-    </row>
-    <row r="7" spans="1:13" ht="29.25" x14ac:dyDescent="0.25">
-      <c r="A7" s="13" t="s">
-        <v>35</v>
-      </c>
-      <c r="B7" s="24" t="s">
-        <v>36</v>
-      </c>
-      <c r="C7" s="18"/>
-      <c r="D7" s="18"/>
-      <c r="E7" s="18"/>
-      <c r="F7" s="18"/>
-      <c r="G7" s="18"/>
-      <c r="H7" s="18"/>
-      <c r="I7" s="18"/>
-      <c r="J7" s="18"/>
-      <c r="K7" s="18"/>
-      <c r="L7" s="18"/>
-      <c r="M7" s="3"/>
-    </row>
-    <row r="8" spans="1:13" ht="129" x14ac:dyDescent="0.25">
-      <c r="A8" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="B8" s="10" t="s">
-        <v>37</v>
-      </c>
-      <c r="C8" s="11" t="s">
-        <v>38</v>
-      </c>
-      <c r="D8" s="10" t="s">
-        <v>39</v>
-      </c>
-      <c r="E8" s="10" t="s">
-        <v>40</v>
-      </c>
-      <c r="F8" s="10" t="s">
-        <v>41</v>
-      </c>
-      <c r="G8" s="11" t="s">
-        <v>42</v>
-      </c>
-      <c r="H8" s="10" t="s">
-        <v>43</v>
-      </c>
-      <c r="I8" s="10" t="s">
-        <v>44</v>
-      </c>
-      <c r="J8" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="K8" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="L8" s="10" t="s">
-        <v>47</v>
-      </c>
-      <c r="M8" s="10" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" ht="29.25" x14ac:dyDescent="0.25">
-      <c r="A9" s="13" t="s">
-        <v>49</v>
-      </c>
-      <c r="B9" s="19" t="s">
-        <v>50</v>
-      </c>
-      <c r="C9" s="18"/>
-      <c r="D9" s="18"/>
-      <c r="E9" s="18"/>
-      <c r="F9" s="18"/>
-      <c r="G9" s="18"/>
-      <c r="H9" s="18"/>
-      <c r="I9" s="18"/>
-      <c r="J9" s="18"/>
-      <c r="K9" s="18"/>
-      <c r="L9" s="18"/>
-      <c r="M9" s="3"/>
-    </row>
-    <row r="10" spans="1:13" ht="157.5" x14ac:dyDescent="0.25">
-      <c r="A10" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="B10" s="10" t="s">
-        <v>51</v>
-      </c>
-      <c r="C10" s="10" t="s">
-        <v>52</v>
-      </c>
-      <c r="D10" s="10" t="s">
-        <v>53</v>
-      </c>
-      <c r="E10" s="10" t="s">
-        <v>54</v>
-      </c>
-      <c r="F10" s="10" t="s">
-        <v>55</v>
-      </c>
-      <c r="G10" s="10" t="s">
-        <v>56</v>
-      </c>
-      <c r="H10" s="10" t="s">
-        <v>57</v>
-      </c>
-      <c r="I10" s="10" t="s">
-        <v>58</v>
-      </c>
-      <c r="J10" s="10" t="s">
-        <v>59</v>
-      </c>
-      <c r="K10" s="10" t="s">
-        <v>60</v>
-      </c>
-      <c r="L10" s="10" t="s">
-        <v>61</v>
-      </c>
-      <c r="M10" s="10" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13" ht="29.25" x14ac:dyDescent="0.25">
-      <c r="A11" s="13" t="s">
-        <v>63</v>
-      </c>
-      <c r="B11" s="19" t="s">
-        <v>64</v>
-      </c>
-      <c r="C11" s="18"/>
-      <c r="D11" s="18"/>
-      <c r="E11" s="18"/>
-      <c r="F11" s="18"/>
-      <c r="G11" s="18"/>
-      <c r="H11" s="18"/>
-      <c r="I11" s="18"/>
-      <c r="J11" s="18"/>
-      <c r="K11" s="18"/>
-      <c r="L11" s="18"/>
-      <c r="M11" s="3"/>
-    </row>
-    <row r="12" spans="1:13" ht="186" x14ac:dyDescent="0.25">
-      <c r="A12" s="14" t="s">
-        <v>20</v>
-      </c>
-      <c r="B12" s="15" t="s">
-        <v>65</v>
-      </c>
-      <c r="C12" s="16" t="s">
-        <v>66</v>
-      </c>
-      <c r="D12" s="16" t="s">
-        <v>67</v>
-      </c>
-      <c r="E12" s="16" t="s">
-        <v>68</v>
-      </c>
-      <c r="F12" s="15" t="s">
-        <v>69</v>
-      </c>
-      <c r="G12" s="15" t="s">
+      <c r="L14" s="7" t="s">
         <v>70</v>
       </c>
-      <c r="H12" s="10" t="s">
+      <c r="M14" s="7" t="s">
         <v>71</v>
-      </c>
-      <c r="I12" s="10" t="s">
-        <v>72</v>
-      </c>
-      <c r="J12" s="10" t="s">
-        <v>73</v>
-      </c>
-      <c r="K12" s="10" t="s">
-        <v>74</v>
-      </c>
-      <c r="L12" s="10" t="s">
-        <v>75</v>
-      </c>
-      <c r="M12" s="10" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13" ht="29.25" x14ac:dyDescent="0.25">
-      <c r="A13" s="13" t="s">
-        <v>77</v>
-      </c>
-      <c r="B13" s="19" t="s">
-        <v>78</v>
-      </c>
-      <c r="C13" s="18"/>
-      <c r="D13" s="18"/>
-      <c r="E13" s="18"/>
-      <c r="F13" s="18"/>
-      <c r="G13" s="18"/>
-      <c r="H13" s="18"/>
-      <c r="I13" s="18"/>
-      <c r="J13" s="18"/>
-      <c r="K13" s="18"/>
-      <c r="L13" s="18"/>
-      <c r="M13" s="3"/>
-    </row>
-    <row r="14" spans="1:13" ht="157.5" x14ac:dyDescent="0.25">
-      <c r="A14" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="B14" s="10" t="s">
-        <v>79</v>
-      </c>
-      <c r="C14" s="10" t="s">
-        <v>80</v>
-      </c>
-      <c r="D14" s="10" t="s">
-        <v>81</v>
-      </c>
-      <c r="E14" s="10" t="s">
-        <v>82</v>
-      </c>
-      <c r="F14" s="10" t="s">
-        <v>83</v>
-      </c>
-      <c r="G14" s="10" t="s">
-        <v>84</v>
-      </c>
-      <c r="H14" s="10" t="s">
-        <v>85</v>
-      </c>
-      <c r="I14" s="10" t="s">
-        <v>86</v>
-      </c>
-      <c r="J14" s="10" t="s">
-        <v>87</v>
-      </c>
-      <c r="K14" s="10" t="s">
-        <v>88</v>
-      </c>
-      <c r="L14" s="10" t="s">
-        <v>89</v>
-      </c>
-      <c r="M14" s="10" t="s">
-        <v>90</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="L1:M1"/>
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="F1:G1"/>
+    <mergeCell ref="H1:I1"/>
+    <mergeCell ref="J1:K1"/>
     <mergeCell ref="B3:M3"/>
     <mergeCell ref="B13:M13"/>
     <mergeCell ref="B4:M4"/>
@@ -1286,12 +1292,6 @@
     <mergeCell ref="B7:M7"/>
     <mergeCell ref="B9:M9"/>
     <mergeCell ref="B11:M11"/>
-    <mergeCell ref="B1:C1"/>
-    <mergeCell ref="D1:E1"/>
-    <mergeCell ref="F1:G1"/>
-    <mergeCell ref="H1:I1"/>
-    <mergeCell ref="J1:K1"/>
-    <mergeCell ref="L1:M1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Added event summary for WarIsComing
</commit_message>
<xml_diff>
--- a/Stories/WarIsComing.xlsx
+++ b/Stories/WarIsComing.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ianch\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\School Related\DECO3801\DECO3801-Synergistiscs\Stories\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B04E654D-AE43-457D-83F4-67D74EFA7D4E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60DFE771-8844-4F3B-874A-9384389259E0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{4C62B3AD-FD19-43ED-8515-0095E96B2E3E}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{4C62B3AD-FD19-43ED-8515-0095E96B2E3E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="102">
   <si>
     <t>MILITARY</t>
   </si>
@@ -309,6 +309,36 @@
   </si>
   <si>
     <t>This is a move that could save our people, but losing the Kingdom.</t>
+  </si>
+  <si>
+    <t>EVENT SUMMARY HEADER</t>
+  </si>
+  <si>
+    <t>ACTION 1 EVENT SUMMARY</t>
+  </si>
+  <si>
+    <t>ACTION 2 EVENT SUMMARY</t>
+  </si>
+  <si>
+    <t>ACTION 3 EVENT SUMMARY</t>
+  </si>
+  <si>
+    <t>ACTION 4 EVENT SUMMARY</t>
+  </si>
+  <si>
+    <t>Despite your best efforts to send some of your men over to negotiate with the neighbouring Kingdom, they refused to listen and is fully intent on taking over your Kingdom.</t>
+  </si>
+  <si>
+    <t>Unfortunately, your decision to wait had allowed for the neighbouring Kingdom to spring a surprise attack on your Kingdom, causing significant damage and leaving you no opportunity to defend or counter attack.</t>
+  </si>
+  <si>
+    <t>You gathered your army to spring a surprise attack on the enemy, catching them off guard and dealing significant damage to their army.</t>
+  </si>
+  <si>
+    <t>By cutting exports of food to the neighbouring Kingdom, you had cut a good percentage of their food supplies. This had affected the ability to support their own people and their war efforts.</t>
+  </si>
+  <si>
+    <t>Abandoning all hope and escaping to your bunker, you had left all your people to die at the hands of the enemy. However, hiding did not matter as enemy spies revealed the location of your bunker, ultimately dying at the hands of the enemy general.</t>
   </si>
 </sst>
 </file>
@@ -483,7 +513,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -525,11 +555,17 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="5" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -544,11 +580,11 @@
     <xf numFmtId="0" fontId="6" fillId="5" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -865,40 +901,40 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C44981BA-9AE4-44E2-B14F-CB86D6B680A9}">
-  <dimension ref="A1:M14"/>
+  <dimension ref="A1:M19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="M14" sqref="M14"/>
+    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1" s="1"/>
-      <c r="B1" s="24" t="s">
+      <c r="B1" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="17"/>
-      <c r="D1" s="25" t="s">
+      <c r="C1" s="16"/>
+      <c r="D1" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="17"/>
-      <c r="F1" s="25" t="s">
+      <c r="E1" s="16"/>
+      <c r="F1" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="17"/>
-      <c r="H1" s="25" t="s">
+      <c r="G1" s="16"/>
+      <c r="H1" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="I1" s="17"/>
-      <c r="J1" s="25" t="s">
+      <c r="I1" s="16"/>
+      <c r="J1" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="K1" s="17"/>
-      <c r="L1" s="25" t="s">
+      <c r="K1" s="16"/>
+      <c r="L1" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="M1" s="17"/>
+      <c r="M1" s="16"/>
     </row>
     <row r="2" spans="1:13" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A2" s="2"/>
@@ -943,39 +979,39 @@
       <c r="A3" s="14" t="s">
         <v>72</v>
       </c>
-      <c r="B3" s="15" t="s">
+      <c r="B3" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="C3" s="16"/>
-      <c r="D3" s="16"/>
-      <c r="E3" s="16"/>
-      <c r="F3" s="16"/>
-      <c r="G3" s="16"/>
-      <c r="H3" s="16"/>
-      <c r="I3" s="16"/>
-      <c r="J3" s="16"/>
-      <c r="K3" s="16"/>
-      <c r="L3" s="16"/>
-      <c r="M3" s="17"/>
+      <c r="C3" s="19"/>
+      <c r="D3" s="19"/>
+      <c r="E3" s="19"/>
+      <c r="F3" s="19"/>
+      <c r="G3" s="19"/>
+      <c r="H3" s="19"/>
+      <c r="I3" s="19"/>
+      <c r="J3" s="19"/>
+      <c r="K3" s="19"/>
+      <c r="L3" s="19"/>
+      <c r="M3" s="16"/>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="b">
         <v>1</v>
       </c>
-      <c r="B4" s="19" t="s">
+      <c r="B4" s="21" t="s">
         <v>80</v>
       </c>
-      <c r="C4" s="16"/>
-      <c r="D4" s="16"/>
-      <c r="E4" s="16"/>
-      <c r="F4" s="16"/>
-      <c r="G4" s="16"/>
-      <c r="H4" s="16"/>
-      <c r="I4" s="16"/>
-      <c r="J4" s="16"/>
-      <c r="K4" s="16"/>
-      <c r="L4" s="16"/>
-      <c r="M4" s="17"/>
+      <c r="C4" s="19"/>
+      <c r="D4" s="19"/>
+      <c r="E4" s="19"/>
+      <c r="F4" s="19"/>
+      <c r="G4" s="19"/>
+      <c r="H4" s="19"/>
+      <c r="I4" s="19"/>
+      <c r="J4" s="19"/>
+      <c r="K4" s="19"/>
+      <c r="L4" s="19"/>
+      <c r="M4" s="16"/>
     </row>
     <row r="5" spans="1:13" ht="180" x14ac:dyDescent="0.3">
       <c r="A5" s="6" t="s">
@@ -1022,39 +1058,39 @@
       <c r="A6" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="B6" s="20" t="s">
+      <c r="B6" s="22" t="s">
         <v>79</v>
       </c>
-      <c r="C6" s="21"/>
-      <c r="D6" s="21"/>
-      <c r="E6" s="21"/>
-      <c r="F6" s="21"/>
-      <c r="G6" s="21"/>
-      <c r="H6" s="21"/>
-      <c r="I6" s="21"/>
-      <c r="J6" s="21"/>
-      <c r="K6" s="21"/>
-      <c r="L6" s="21"/>
-      <c r="M6" s="22"/>
+      <c r="C6" s="23"/>
+      <c r="D6" s="23"/>
+      <c r="E6" s="23"/>
+      <c r="F6" s="23"/>
+      <c r="G6" s="23"/>
+      <c r="H6" s="23"/>
+      <c r="I6" s="23"/>
+      <c r="J6" s="23"/>
+      <c r="K6" s="23"/>
+      <c r="L6" s="23"/>
+      <c r="M6" s="24"/>
     </row>
     <row r="7" spans="1:13" ht="28.2" x14ac:dyDescent="0.3">
       <c r="A7" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="B7" s="23" t="s">
+      <c r="B7" s="25" t="s">
         <v>28</v>
       </c>
-      <c r="C7" s="16"/>
-      <c r="D7" s="16"/>
-      <c r="E7" s="16"/>
-      <c r="F7" s="16"/>
-      <c r="G7" s="16"/>
-      <c r="H7" s="16"/>
-      <c r="I7" s="16"/>
-      <c r="J7" s="16"/>
-      <c r="K7" s="16"/>
-      <c r="L7" s="16"/>
-      <c r="M7" s="17"/>
+      <c r="C7" s="19"/>
+      <c r="D7" s="19"/>
+      <c r="E7" s="19"/>
+      <c r="F7" s="19"/>
+      <c r="G7" s="19"/>
+      <c r="H7" s="19"/>
+      <c r="I7" s="19"/>
+      <c r="J7" s="19"/>
+      <c r="K7" s="19"/>
+      <c r="L7" s="19"/>
+      <c r="M7" s="16"/>
     </row>
     <row r="8" spans="1:13" ht="138.6" x14ac:dyDescent="0.3">
       <c r="A8" s="6" t="s">
@@ -1101,20 +1137,20 @@
       <c r="A9" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="B9" s="18" t="s">
+      <c r="B9" s="20" t="s">
         <v>41</v>
       </c>
-      <c r="C9" s="16"/>
-      <c r="D9" s="16"/>
-      <c r="E9" s="16"/>
-      <c r="F9" s="16"/>
-      <c r="G9" s="16"/>
-      <c r="H9" s="16"/>
-      <c r="I9" s="16"/>
-      <c r="J9" s="16"/>
-      <c r="K9" s="16"/>
-      <c r="L9" s="16"/>
-      <c r="M9" s="17"/>
+      <c r="C9" s="19"/>
+      <c r="D9" s="19"/>
+      <c r="E9" s="19"/>
+      <c r="F9" s="19"/>
+      <c r="G9" s="19"/>
+      <c r="H9" s="19"/>
+      <c r="I9" s="19"/>
+      <c r="J9" s="19"/>
+      <c r="K9" s="19"/>
+      <c r="L9" s="19"/>
+      <c r="M9" s="16"/>
     </row>
     <row r="10" spans="1:13" ht="152.4" x14ac:dyDescent="0.3">
       <c r="A10" s="6" t="s">
@@ -1161,20 +1197,20 @@
       <c r="A11" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="B11" s="18" t="s">
+      <c r="B11" s="20" t="s">
         <v>52</v>
       </c>
-      <c r="C11" s="16"/>
-      <c r="D11" s="16"/>
-      <c r="E11" s="16"/>
-      <c r="F11" s="16"/>
-      <c r="G11" s="16"/>
-      <c r="H11" s="16"/>
-      <c r="I11" s="16"/>
-      <c r="J11" s="16"/>
-      <c r="K11" s="16"/>
-      <c r="L11" s="16"/>
-      <c r="M11" s="17"/>
+      <c r="C11" s="19"/>
+      <c r="D11" s="19"/>
+      <c r="E11" s="19"/>
+      <c r="F11" s="19"/>
+      <c r="G11" s="19"/>
+      <c r="H11" s="19"/>
+      <c r="I11" s="19"/>
+      <c r="J11" s="19"/>
+      <c r="K11" s="19"/>
+      <c r="L11" s="19"/>
+      <c r="M11" s="16"/>
     </row>
     <row r="12" spans="1:13" ht="180" x14ac:dyDescent="0.3">
       <c r="A12" s="11" t="s">
@@ -1221,20 +1257,20 @@
       <c r="A13" s="10" t="s">
         <v>61</v>
       </c>
-      <c r="B13" s="18" t="s">
+      <c r="B13" s="20" t="s">
         <v>62</v>
       </c>
-      <c r="C13" s="16"/>
-      <c r="D13" s="16"/>
-      <c r="E13" s="16"/>
-      <c r="F13" s="16"/>
-      <c r="G13" s="16"/>
-      <c r="H13" s="16"/>
-      <c r="I13" s="16"/>
-      <c r="J13" s="16"/>
-      <c r="K13" s="16"/>
-      <c r="L13" s="16"/>
-      <c r="M13" s="17"/>
+      <c r="C13" s="19"/>
+      <c r="D13" s="19"/>
+      <c r="E13" s="19"/>
+      <c r="F13" s="19"/>
+      <c r="G13" s="19"/>
+      <c r="H13" s="19"/>
+      <c r="I13" s="19"/>
+      <c r="J13" s="19"/>
+      <c r="K13" s="19"/>
+      <c r="L13" s="19"/>
+      <c r="M13" s="16"/>
     </row>
     <row r="14" spans="1:13" ht="152.4" x14ac:dyDescent="0.3">
       <c r="A14" s="6" t="s">
@@ -1277,14 +1313,108 @@
         <v>71</v>
       </c>
     </row>
+    <row r="15" spans="1:13" ht="55.2" x14ac:dyDescent="0.3">
+      <c r="A15" s="26" t="s">
+        <v>92</v>
+      </c>
+      <c r="B15" s="27" t="s">
+        <v>97</v>
+      </c>
+      <c r="C15" s="19"/>
+      <c r="D15" s="19"/>
+      <c r="E15" s="19"/>
+      <c r="F15" s="19"/>
+      <c r="G15" s="19"/>
+      <c r="H15" s="19"/>
+      <c r="I15" s="19"/>
+      <c r="J15" s="19"/>
+      <c r="K15" s="19"/>
+      <c r="L15" s="19"/>
+      <c r="M15" s="16"/>
+    </row>
+    <row r="16" spans="1:13" ht="55.2" x14ac:dyDescent="0.3">
+      <c r="A16" s="26" t="s">
+        <v>93</v>
+      </c>
+      <c r="B16" s="27" t="s">
+        <v>98</v>
+      </c>
+      <c r="C16" s="19"/>
+      <c r="D16" s="19"/>
+      <c r="E16" s="19"/>
+      <c r="F16" s="19"/>
+      <c r="G16" s="19"/>
+      <c r="H16" s="19"/>
+      <c r="I16" s="19"/>
+      <c r="J16" s="19"/>
+      <c r="K16" s="19"/>
+      <c r="L16" s="19"/>
+      <c r="M16" s="16"/>
+    </row>
+    <row r="17" spans="1:13" ht="55.2" x14ac:dyDescent="0.3">
+      <c r="A17" s="26" t="s">
+        <v>94</v>
+      </c>
+      <c r="B17" s="27" t="s">
+        <v>99</v>
+      </c>
+      <c r="C17" s="19"/>
+      <c r="D17" s="19"/>
+      <c r="E17" s="19"/>
+      <c r="F17" s="19"/>
+      <c r="G17" s="19"/>
+      <c r="H17" s="19"/>
+      <c r="I17" s="19"/>
+      <c r="J17" s="19"/>
+      <c r="K17" s="19"/>
+      <c r="L17" s="19"/>
+      <c r="M17" s="16"/>
+    </row>
+    <row r="18" spans="1:13" ht="55.2" x14ac:dyDescent="0.3">
+      <c r="A18" s="26" t="s">
+        <v>95</v>
+      </c>
+      <c r="B18" s="27" t="s">
+        <v>100</v>
+      </c>
+      <c r="C18" s="19"/>
+      <c r="D18" s="19"/>
+      <c r="E18" s="19"/>
+      <c r="F18" s="19"/>
+      <c r="G18" s="19"/>
+      <c r="H18" s="19"/>
+      <c r="I18" s="19"/>
+      <c r="J18" s="19"/>
+      <c r="K18" s="19"/>
+      <c r="L18" s="19"/>
+      <c r="M18" s="16"/>
+    </row>
+    <row r="19" spans="1:13" ht="55.2" x14ac:dyDescent="0.3">
+      <c r="A19" s="26" t="s">
+        <v>96</v>
+      </c>
+      <c r="B19" s="27" t="s">
+        <v>101</v>
+      </c>
+      <c r="C19" s="19"/>
+      <c r="D19" s="19"/>
+      <c r="E19" s="19"/>
+      <c r="F19" s="19"/>
+      <c r="G19" s="19"/>
+      <c r="H19" s="19"/>
+      <c r="I19" s="19"/>
+      <c r="J19" s="19"/>
+      <c r="K19" s="19"/>
+      <c r="L19" s="19"/>
+      <c r="M19" s="16"/>
+    </row>
   </sheetData>
-  <mergeCells count="13">
-    <mergeCell ref="L1:M1"/>
-    <mergeCell ref="B1:C1"/>
-    <mergeCell ref="D1:E1"/>
-    <mergeCell ref="F1:G1"/>
-    <mergeCell ref="H1:I1"/>
-    <mergeCell ref="J1:K1"/>
+  <mergeCells count="18">
+    <mergeCell ref="B15:M15"/>
+    <mergeCell ref="B16:M16"/>
+    <mergeCell ref="B17:M17"/>
+    <mergeCell ref="B18:M18"/>
+    <mergeCell ref="B19:M19"/>
     <mergeCell ref="B3:M3"/>
     <mergeCell ref="B13:M13"/>
     <mergeCell ref="B4:M4"/>
@@ -1292,6 +1422,12 @@
     <mergeCell ref="B7:M7"/>
     <mergeCell ref="B9:M9"/>
     <mergeCell ref="B11:M11"/>
+    <mergeCell ref="L1:M1"/>
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="F1:G1"/>
+    <mergeCell ref="H1:I1"/>
+    <mergeCell ref="J1:K1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>